<commit_message>
Imports Excel sheet of student data
</commit_message>
<xml_diff>
--- a/MyList.xlsx
+++ b/MyList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m/code/firstyearwriting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EFCF2F9-6FB7-CC41-B6DF-D0AF5B523B70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8709AC-86AC-334E-9A36-8CAE6EDA3DA0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15960" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Home - 2021" sheetId="2" r:id="rId1"/>
@@ -20,32 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="241">
   <si>
     <t>2021</t>
   </si>
   <si>
-    <t>Section</t>
-  </si>
-  <si>
-    <t>Last</t>
-  </si>
-  <si>
-    <t>First</t>
-  </si>
-  <si>
-    <t>Middle</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Accommodations</t>
-  </si>
-  <si>
-    <t>Achieve</t>
-  </si>
-  <si>
     <t>C5</t>
   </si>
   <si>
@@ -75,9 +54,6 @@
     <t>In Person</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>C4</t>
   </si>
   <si>
@@ -107,9 +83,6 @@
     </r>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Bhatia</t>
   </si>
   <si>
@@ -1153,23 +1126,14 @@
     </r>
   </si>
   <si>
-    <t>LfA</t>
-  </si>
-  <si>
-    <t>Goesby</t>
-  </si>
-  <si>
-    <t>StudentID</t>
-  </si>
-  <si>
-    <t>Phone</t>
+    <t>1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -1188,12 +1152,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color indexed="12"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
@@ -1204,7 +1162,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1213,68 +1171,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="16"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="14"/>
-      </left>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="14"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="14"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="14"/>
-      </right>
-      <top style="thin">
-        <color indexed="14"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1313,47 +1220,38 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2516,10 +2414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="22.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2533,56 +2431,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="29.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-    </row>
-    <row r="2" spans="1:11" ht="32.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+    </row>
+    <row r="2" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" ht="103" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -2592,1374 +2482,1345 @@
       <c r="C3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="E3" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="103" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="8" t="s">
+      <c r="C4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="H4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="E5" s="8"/>
+      <c r="F5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="8" t="s">
+      <c r="G5" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="12" t="s">
+      <c r="H5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="6"/>
+      <c r="K6" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="B10" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="12" t="s">
+      <c r="B11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="8"/>
+      <c r="J11" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="K11" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="12" t="s">
+      <c r="B12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="B14" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" s="9"/>
-      <c r="K7" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="8" t="s">
+      <c r="I15" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+    </row>
+    <row r="16" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="13" t="s">
+      <c r="B17" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+    </row>
+    <row r="23" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="11"/>
-      <c r="J12" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-    </row>
-    <row r="17" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="12" t="s">
+      <c r="D31" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E31" s="8"/>
+      <c r="F31" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+    </row>
+    <row r="32" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-    </row>
-    <row r="18" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="12" t="s">
+      <c r="B32" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E32" s="6"/>
+      <c r="F32" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+    </row>
+    <row r="33" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E33" s="8"/>
+      <c r="F33" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="J33" s="8"/>
+      <c r="K33" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="E34" s="6"/>
+      <c r="F34" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="H19" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" s="10" t="s">
+      <c r="B35" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="D36" s="6"/>
+      <c r="E36" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="H36" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="12" t="s">
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+    </row>
+    <row r="37" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D37" s="8"/>
+      <c r="E37" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+    </row>
+    <row r="38" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+    </row>
+    <row r="39" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="E40" s="6"/>
+      <c r="F40" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="H21" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-    </row>
-    <row r="22" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-    </row>
-    <row r="24" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="12" t="s">
+      <c r="B41" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D41" s="8"/>
+      <c r="E41" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="J41" s="8"/>
+      <c r="K41" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="E42" s="6"/>
+      <c r="F42" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
+    </row>
+    <row r="43" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="D43" s="8"/>
+      <c r="E43" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="D44" s="6"/>
+      <c r="E44" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I44" s="6"/>
+      <c r="J44" s="6"/>
+      <c r="K44" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+    </row>
+    <row r="46" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="E46" s="6"/>
+      <c r="F46" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="H46" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6"/>
+      <c r="K46" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="D47" s="8"/>
+      <c r="E47" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D48" s="6"/>
+      <c r="E48" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="H48" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I48" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="J48" s="6"/>
+      <c r="K48" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="H25" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="H26" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="H29" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="H31" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="E32" s="11"/>
-      <c r="F32" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="H32" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-    </row>
-    <row r="33" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="E33" s="9"/>
-      <c r="F33" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="H33" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-    </row>
-    <row r="34" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="E34" s="11"/>
-      <c r="F34" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="H34" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="J34" s="11"/>
-      <c r="K34" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="E35" s="9"/>
-      <c r="F35" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="H35" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="H36" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="D37" s="9"/>
-      <c r="E37" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="H37" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
-    </row>
-    <row r="38" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="H38" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-    </row>
-    <row r="39" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="G39" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="H39" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I39" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
-    </row>
-    <row r="40" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="G40" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="H40" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="E41" s="9"/>
-      <c r="F41" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="G41" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="H41" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="I41" s="9"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D42" s="11"/>
-      <c r="E42" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="G42" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="H42" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="I42" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="J42" s="11"/>
-      <c r="K42" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="E43" s="9"/>
-      <c r="F43" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="G43" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="H43" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
-    </row>
-    <row r="44" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="D44" s="11"/>
-      <c r="E44" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="G44" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="H44" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I44" s="11"/>
-      <c r="J44" s="11"/>
-      <c r="K44" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="D45" s="9"/>
-      <c r="E45" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="F45" s="12" t="s">
-        <v>223</v>
-      </c>
-      <c r="G45" s="12" t="s">
-        <v>224</v>
-      </c>
-      <c r="H45" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I45" s="9"/>
-      <c r="J45" s="9"/>
-      <c r="K45" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="G46" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="H46" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="11"/>
-    </row>
-    <row r="47" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D47" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="E47" s="9"/>
-      <c r="F47" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="G47" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="H47" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B48" s="10" t="s">
+      <c r="B49" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C49" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="D48" s="11"/>
-      <c r="E48" s="8" t="s">
+      <c r="D49" s="8"/>
+      <c r="E49" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="F48" s="8" t="s">
+      <c r="F49" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="G48" s="8" t="s">
+      <c r="G49" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="H48" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="D49" s="9"/>
-      <c r="E49" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="F49" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="G49" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="H49" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I49" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="J49" s="9"/>
-      <c r="K49" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B50" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="D50" s="11"/>
-      <c r="E50" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="G50" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="H50" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="8" t="s">
-        <v>23</v>
+      <c r="H49" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3967,54 +3828,54 @@
     <mergeCell ref="A1:K1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="G4" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="G5" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="G6" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="G7" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="G8" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="G9" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="G10" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="G11" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="G12" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="G13" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="G14" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="G15" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="G16" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="G17" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="G18" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="G19" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="G20" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="G21" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="G22" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="G23" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="G24" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="G25" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="G26" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="G27" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="G28" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
-    <hyperlink ref="G29" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="G30" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="G31" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="G32" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="G33" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="G34" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="G35" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="G36" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="G37" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="G38" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="G39" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink ref="G40" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
-    <hyperlink ref="G41" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
-    <hyperlink ref="G42" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
-    <hyperlink ref="G43" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink ref="G44" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
-    <hyperlink ref="G45" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink ref="G46" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink ref="G47" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
-    <hyperlink ref="G48" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink ref="G49" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink ref="G50" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="G9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="G10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="G11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="G12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="G13" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="G14" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="G15" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="G16" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="G17" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="G18" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="G19" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="G20" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="G21" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="G22" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="G23" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="G24" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="G25" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="G26" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="G27" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="G28" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="G29" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="G30" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="G31" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="G32" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="G33" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="G34" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="G35" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="G36" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="G37" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="G38" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="G39" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="G40" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="G41" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="G42" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="G43" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="G44" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="G45" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="G46" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="G47" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="G48" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="G49" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup scale="72" orientation="portrait"/>

</xml_diff>